<commit_message>
Completed hill climber and evaluation
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath-my.sharepoint.com/personal/jjb19182_uni_strath_ac_uk/Documents/CS547 - Advanced Topics in Software Engineering/Assignments/Assignment 2 - Test Case Prioritization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive - University of Strathclyde\CS547 - Advanced Topics in Software Engineering\Assignments\Assignment 2 - Test Case Prioritization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEC165B0-06D6-47E5-903B-27B9D96F2DBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{BEC165B0-06D6-47E5-903B-27B9D96F2DBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0F9B567F-D0AA-4DF3-8B29-3919CE950D48}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C1EDD83C-0520-454A-AC14-AC91E10B4667}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>GA with small</t>
   </si>
@@ -88,16 +88,42 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>GA outperform random with small</t>
+  </si>
+  <si>
+    <t>GA outperform hill climber with small</t>
+  </si>
+  <si>
+    <t>GA outperform random with big</t>
+  </si>
+  <si>
+    <t>GA outperform hill climber with big</t>
+  </si>
+  <si>
+    <t>Hill climber outperform random with small</t>
+  </si>
+  <si>
+    <t>Hill climber outperform random with big</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,7 +137,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -119,14 +145,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,60 +478,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5548733D-DBF2-43FD-8BEC-E4C90DDB9F57}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="39.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:19" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2">
@@ -537,9 +582,15 @@
         <f>AVERAGE(C2:L2)</f>
         <v>46.3</v>
       </c>
+      <c r="R2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:19" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3">
@@ -584,9 +635,16 @@
         <f>AVERAGE(C3:L3)</f>
         <v>51.8</v>
       </c>
+      <c r="R3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0.4</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="4" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5">
@@ -620,20 +678,26 @@
         <v>161</v>
       </c>
       <c r="N5">
-        <f t="shared" ref="N4:N6" si="0">MIN(C5:L5)</f>
+        <f t="shared" ref="N5:N9" si="0">MIN(C5:L5)</f>
         <v>6</v>
       </c>
       <c r="O5">
-        <f t="shared" ref="O4:O6" si="1">MAX(C5:L5)</f>
+        <f t="shared" ref="O5:O9" si="1">MAX(C5:L5)</f>
         <v>161</v>
       </c>
       <c r="P5">
-        <f t="shared" ref="P4:P6" si="2">AVERAGE(C5:L5)</f>
+        <f t="shared" ref="P5:P9" si="2">AVERAGE(C5:L5)</f>
         <v>66.8</v>
       </c>
+      <c r="R5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:19" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6">
@@ -678,17 +742,121 @@
         <f t="shared" si="2"/>
         <v>90.3</v>
       </c>
+      <c r="R6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.6</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="7" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C8">
+        <v>227</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>29</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>53</v>
+      </c>
+      <c r="H8">
+        <v>79</v>
+      </c>
+      <c r="I8">
+        <v>19</v>
+      </c>
+      <c r="J8">
+        <v>51</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>34</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>227</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>51.9</v>
+      </c>
+      <c r="R8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.6</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:19" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C9">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>64</v>
+      </c>
+      <c r="F9">
+        <v>76</v>
+      </c>
+      <c r="G9">
+        <v>104</v>
+      </c>
+      <c r="H9">
+        <v>45</v>
+      </c>
+      <c r="I9">
+        <v>22</v>
+      </c>
+      <c r="J9">
+        <v>80</v>
+      </c>
+      <c r="K9">
+        <v>63</v>
+      </c>
+      <c r="L9">
+        <v>144</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="2"/>
+        <v>62.9</v>
+      </c>
+      <c r="R9" t="s">
+        <v>24</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.6</v>
+      </c>
     </row>
+    <row r="10" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>